<commit_message>
Graphs for polynomials are added
</commit_message>
<xml_diff>
--- a/resultBook.xlsx
+++ b/resultBook.xlsx
@@ -246,28 +246,34 @@
                   <c:v>0.7936507936507936</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7964671443145541</c:v>
+                  <c:v>0.7985175398975912</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.7906774682135751</c:v>
+                  <c:v>0.7999470240275934</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.7814381039512455</c:v>
+                  <c:v>0.7968687010880957</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.7778418286371996</c:v>
+                  <c:v>0.7880999397162711</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.7922867964911235</c:v>
+                  <c:v>0.7723411720772755</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.8402330979295879</c:v>
+                  <c:v>0.7481814851195527</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.9479979101655877</c:v>
+                  <c:v>0.7141198053212</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.3008905245733196</c:v>
+                  <c:v>0.6686209550437986</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.6102593894050423</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5379563171798417</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -507,28 +513,34 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.49595820946638686</c:v>
+                  <c:v>0.5004777314014607</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.4967414819875809</c:v>
+                  <c:v>0.5069132785551892</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.503710830465092</c:v>
+                  <c:v>0.519317406125767</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5178455560495622</c:v>
+                  <c:v>0.5376301729805513</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5396245194667215</c:v>
+                  <c:v>0.5616569204523728</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5688239232760537</c:v>
+                  <c:v>0.5909523851306558</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.6041300036879443</c:v>
+                  <c:v>0.6247238645063495</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.639659025138353</c:v>
+                  <c:v>0.6620723359362585</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.7036605676547337</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.7579368499408234</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -768,28 +780,34 @@
                   <c:v>0.6627906976744186</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6628295253534962</c:v>
+                  <c:v>0.6625592712483745</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6630062184405032</c:v>
+                  <c:v>0.6577605454001819</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6630935352519138</c:v>
+                  <c:v>0.6478621622318</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.6639640597683856</c:v>
+                  <c:v>0.6323665658068801</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.6679471918592746</c:v>
+                  <c:v>0.610897288747511</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.6795751510383745</c:v>
+                  <c:v>0.5833421956229687</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.7058480046218535</c:v>
+                  <c:v>0.5500761126945722</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.7097351459340132</c:v>
+                  <c:v>0.512299989687191</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.4725673618374788</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.4356465931125301</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1029,28 +1047,34 @@
                   <c:v>0.5581395348837209</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5099930956620924</c:v>
+                  <c:v>0.5193952492514508</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.45711599013229653</c:v>
+                  <c:v>0.47807060976512555</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.406077043337168</c:v>
+                  <c:v>0.43276393224764764</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3647031765197393</c:v>
+                  <c:v>0.38179996237145425</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.3406899078713495</c:v>
+                  <c:v>0.32320010514409264</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.3404923255650808</c:v>
+                  <c:v>0.25467405943894467</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.3716256617973446</c:v>
+                  <c:v>0.17366269217231584</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.4962748986478847</c:v>
+                  <c:v>0.07755608595454938</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.03546866382286415</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.16370879988422202</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1290,28 +1314,34 @@
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.302007062833514</c:v>
+                  <c:v>0.30142108200324147</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.354252308579409</c:v>
+                  <c:v>0.3527639360354631</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.4075166639982712</c:v>
+                  <c:v>0.40412602621681165</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.46157506244695784</c:v>
+                  <c:v>0.4556039878270791</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5151709258931287</c:v>
+                  <c:v>0.5071112501299861</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5643871840916997</c:v>
+                  <c:v>0.5580512162527507</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5984377770153663</c:v>
+                  <c:v>0.6067936876235762</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.6588468883790187</c:v>
+                  <c:v>0.6499005734600232</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.6810684722887468</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.6898376981702953</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1551,28 +1581,34 @@
                   <c:v>0.851063829787234</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8392883244104472</c:v>
+                  <c:v>0.8392756871350325</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8280065221462676</c:v>
+                  <c:v>0.8298855210392078</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.8170804974956404</c:v>
+                  <c:v>0.8233155257857421</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.8065108131163878</c:v>
+                  <c:v>0.8201712361188181</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.7972182114201611</c:v>
+                  <c:v>0.8213324531964666</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.7914882516171524</c:v>
+                  <c:v>0.8280820115578699</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.7926615351408683</c:v>
+                  <c:v>0.842282767630592</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.8105991436636295</c:v>
+                  <c:v>0.866601550374608</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9047093696348399</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9610773304917004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1812,28 +1848,34 @@
                   <c:v>0.8333333333333334</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8264785300783741</c:v>
+                  <c:v>0.829903494774499</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8245404310007842</c:v>
+                  <c:v>0.8315816087477425</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.8283598582102457</c:v>
+                  <c:v>0.8397982646064193</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.8386558104572164</c:v>
+                  <c:v>0.8559663835764175</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.8561624135773453</c:v>
+                  <c:v>0.8815150662730444</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.8817507540953703</c:v>
+                  <c:v>0.9179192194199888</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.9162287135217655</c:v>
+                  <c:v>0.9667009099755334</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.9589327580386456</c:v>
+                  <c:v>1.0293618520063987</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.107200167791253</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.2010108667157728</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2073,28 +2115,34 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.09997666402937262</c:v>
+                  <c:v>-0.09999558493425532</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.1999575110026547</c:v>
+                  <c:v>-0.19990121713088746</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.2999219231562071</c:v>
+                  <c:v>-0.29968577862942636</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.3998419320349996</c:v>
+                  <c:v>-0.39934315648513025</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.49969315389369456</c:v>
+                  <c:v>-0.4988979508479157</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.5994563648821072</c:v>
+                  <c:v>-0.598384589357363</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.6990186661349361</c:v>
+                  <c:v>-0.697794786347635</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.7977693459062923</c:v>
+                  <c:v>-0.7969972153746345</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.8956217756965511</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.9928278992206233</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2334,28 +2382,34 @@
                   <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7840219905118383</c:v>
+                  <c:v>0.7804842244320525</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.865658675233345</c:v>
+                  <c:v>0.8619827917663819</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.9429829311968112</c:v>
+                  <c:v>0.9453887806576081</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0141398597649318</c:v>
+                  <c:v>1.031760661783467</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0778066029841282</c:v>
+                  <c:v>1.1224237026840023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1329948591318892</c:v>
+                  <c:v>1.2190347556417933</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.1880844954657954</c:v>
+                  <c:v>1.3234177912581395</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.3635740929951088</c:v>
+                  <c:v>1.4366816849518937</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5567425212427146</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.6744069080591903</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2595,28 +2649,34 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5855114907477058</c:v>
+                  <c:v>0.5877714784914168</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6707727835243567</c:v>
+                  <c:v>0.6755758722216769</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.7560569160663633</c:v>
+                  <c:v>0.7638295634098229</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.841821797979485</c:v>
+                  <c:v>0.852995107631085</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.9287355349196834</c:v>
+                  <c:v>0.9435610710894989</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0177066446734158</c:v>
+                  <c:v>1.0360147936549124</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.1095734901044734</c:v>
+                  <c:v>1.1308013356575952</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.2002074504988725</c:v>
+                  <c:v>1.2282618001805785</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.3285379784934344</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.4313638577160734</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3149,34 +3209,34 @@
         <v>0.7936507936507936</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7964671443145541</v>
+        <v>0.7985175398975912</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7906774682135751</v>
+        <v>0.7999470240275934</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7814381039512455</v>
+        <v>0.7968687010880957</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7778418286371996</v>
+        <v>0.7880999397162711</v>
       </c>
       <c r="G2" t="n">
-        <v>0.7922867964911235</v>
+        <v>0.7723411720772755</v>
       </c>
       <c r="H2" t="n">
-        <v>0.8402330979295879</v>
+        <v>0.7481814851195527</v>
       </c>
       <c r="I2" t="n">
-        <v>0.9479979101655877</v>
+        <v>0.7141198053212</v>
       </c>
       <c r="J2" t="n">
-        <v>1.3008905245733196</v>
-      </c>
-      <c r="K2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="L2" t="e">
-        <v>#NUM!</v>
+        <v>0.6686209550437986</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.6102593894050423</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.5379563171798417</v>
       </c>
     </row>
     <row r="3">
@@ -3187,34 +3247,34 @@
         <v>0.6627906976744186</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6628295253534962</v>
+        <v>0.6625592712483745</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6630062184405032</v>
+        <v>0.6577605454001819</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6630935352519138</v>
+        <v>0.6478621622318</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6639640597683856</v>
+        <v>0.6323665658068801</v>
       </c>
       <c r="G3" t="n">
-        <v>0.6679471918592746</v>
+        <v>0.610897288747511</v>
       </c>
       <c r="H3" t="n">
-        <v>0.6795751510383745</v>
+        <v>0.5833421956229687</v>
       </c>
       <c r="I3" t="n">
-        <v>0.7058480046218535</v>
+        <v>0.5500761126945722</v>
       </c>
       <c r="J3" t="n">
-        <v>0.7097351459340132</v>
-      </c>
-      <c r="K3" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="L3" t="e">
-        <v>#NUM!</v>
+        <v>0.512299989687191</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.4725673618374788</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.4356465931125301</v>
       </c>
     </row>
     <row r="4">
@@ -3225,34 +3285,34 @@
         <v>0.5581395348837209</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5099930956620924</v>
+        <v>0.5193952492514508</v>
       </c>
       <c r="D4" t="n">
-        <v>0.45711599013229653</v>
+        <v>0.47807060976512555</v>
       </c>
       <c r="E4" t="n">
-        <v>0.406077043337168</v>
+        <v>0.43276393224764764</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3647031765197393</v>
+        <v>0.38179996237145425</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3406899078713495</v>
+        <v>0.32320010514409264</v>
       </c>
       <c r="H4" t="n">
-        <v>0.3404923255650808</v>
+        <v>0.25467405943894467</v>
       </c>
       <c r="I4" t="n">
-        <v>0.3716256617973446</v>
+        <v>0.17366269217231584</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4962748986478847</v>
-      </c>
-      <c r="K4" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="L4" t="e">
-        <v>#NUM!</v>
+        <v>0.07755608595454938</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-0.03546866382286415</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-0.16370879988422202</v>
       </c>
     </row>
     <row r="5">
@@ -3263,34 +3323,34 @@
         <v>0.25</v>
       </c>
       <c r="C5" t="n">
-        <v>0.302007062833514</v>
+        <v>0.30142108200324147</v>
       </c>
       <c r="D5" t="n">
-        <v>0.354252308579409</v>
+        <v>0.3527639360354631</v>
       </c>
       <c r="E5" t="n">
-        <v>0.4075166639982712</v>
+        <v>0.40412602621681165</v>
       </c>
       <c r="F5" t="n">
-        <v>0.46157506244695784</v>
+        <v>0.4556039878270791</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5151709258931287</v>
+        <v>0.5071112501299861</v>
       </c>
       <c r="H5" t="n">
-        <v>0.5643871840916997</v>
+        <v>0.5580512162527507</v>
       </c>
       <c r="I5" t="n">
-        <v>0.5984377770153663</v>
+        <v>0.6067936876235762</v>
       </c>
       <c r="J5" t="n">
-        <v>0.6588468883790187</v>
-      </c>
-      <c r="K5" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="L5" t="e">
-        <v>#NUM!</v>
+        <v>0.6499005734600232</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.6810684722887468</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.6898376981702953</v>
       </c>
     </row>
     <row r="6">
@@ -3301,34 +3361,34 @@
         <v>0.851063829787234</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8392883244104472</v>
+        <v>0.8392756871350325</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8280065221462676</v>
+        <v>0.8298855210392078</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8170804974956404</v>
+        <v>0.8233155257857421</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8065108131163878</v>
+        <v>0.8201712361188181</v>
       </c>
       <c r="G6" t="n">
-        <v>0.7972182114201611</v>
+        <v>0.8213324531964666</v>
       </c>
       <c r="H6" t="n">
-        <v>0.7914882516171524</v>
+        <v>0.8280820115578699</v>
       </c>
       <c r="I6" t="n">
-        <v>0.7926615351408683</v>
+        <v>0.842282767630592</v>
       </c>
       <c r="J6" t="n">
-        <v>0.8105991436636295</v>
-      </c>
-      <c r="K6" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="L6" t="e">
-        <v>#NUM!</v>
+        <v>0.866601550374608</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.9047093696348399</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.9610773304917004</v>
       </c>
     </row>
     <row r="7">
@@ -3339,34 +3399,34 @@
         <v>0.8333333333333334</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8264785300783741</v>
+        <v>0.829903494774499</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8245404310007842</v>
+        <v>0.8315816087477425</v>
       </c>
       <c r="E7" t="n">
-        <v>0.8283598582102457</v>
+        <v>0.8397982646064193</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8386558104572164</v>
+        <v>0.8559663835764175</v>
       </c>
       <c r="G7" t="n">
-        <v>0.8561624135773453</v>
+        <v>0.8815150662730444</v>
       </c>
       <c r="H7" t="n">
-        <v>0.8817507540953703</v>
+        <v>0.9179192194199888</v>
       </c>
       <c r="I7" t="n">
-        <v>0.9162287135217655</v>
+        <v>0.9667009099755334</v>
       </c>
       <c r="J7" t="n">
-        <v>0.9589327580386456</v>
-      </c>
-      <c r="K7" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="L7" t="e">
-        <v>#NUM!</v>
+        <v>1.0293618520063987</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1.107200167791253</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1.2010108667157728</v>
       </c>
     </row>
     <row r="8">
@@ -3377,34 +3437,34 @@
         <v>0.0</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.09997666402937262</v>
+        <v>-0.09999558493425532</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.1999575110026547</v>
+        <v>-0.19990121713088746</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.2999219231562071</v>
+        <v>-0.29968577862942636</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.3998419320349996</v>
+        <v>-0.39934315648513025</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.49969315389369456</v>
+        <v>-0.4988979508479157</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.5994563648821072</v>
+        <v>-0.598384589357363</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.6990186661349361</v>
+        <v>-0.697794786347635</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.7977693459062923</v>
-      </c>
-      <c r="K8" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="L8" t="e">
-        <v>#NUM!</v>
+        <v>-0.7969972153746345</v>
+      </c>
+      <c r="K8" t="n">
+        <v>-0.8956217756965511</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-0.9928278992206233</v>
       </c>
     </row>
     <row r="9">
@@ -3415,34 +3475,34 @@
         <v>0.7</v>
       </c>
       <c r="C9" t="n">
-        <v>0.7840219905118383</v>
+        <v>0.7804842244320525</v>
       </c>
       <c r="D9" t="n">
-        <v>0.865658675233345</v>
+        <v>0.8619827917663819</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9429829311968112</v>
+        <v>0.9453887806576081</v>
       </c>
       <c r="F9" t="n">
-        <v>1.0141398597649318</v>
+        <v>1.031760661783467</v>
       </c>
       <c r="G9" t="n">
-        <v>1.0778066029841282</v>
+        <v>1.1224237026840023</v>
       </c>
       <c r="H9" t="n">
-        <v>1.1329948591318892</v>
+        <v>1.2190347556417933</v>
       </c>
       <c r="I9" t="n">
-        <v>1.1880844954657954</v>
+        <v>1.3234177912581395</v>
       </c>
       <c r="J9" t="n">
-        <v>1.3635740929951088</v>
-      </c>
-      <c r="K9" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="L9" t="e">
-        <v>#NUM!</v>
+        <v>1.4366816849518937</v>
+      </c>
+      <c r="K9" t="n">
+        <v>1.5567425212427146</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1.6744069080591903</v>
       </c>
     </row>
     <row r="10">
@@ -3453,34 +3513,34 @@
         <v>0.5</v>
       </c>
       <c r="C10" t="n">
-        <v>0.5855114907477058</v>
+        <v>0.5877714784914168</v>
       </c>
       <c r="D10" t="n">
-        <v>0.6707727835243567</v>
+        <v>0.6755758722216769</v>
       </c>
       <c r="E10" t="n">
-        <v>0.7560569160663633</v>
+        <v>0.7638295634098229</v>
       </c>
       <c r="F10" t="n">
-        <v>0.841821797979485</v>
+        <v>0.852995107631085</v>
       </c>
       <c r="G10" t="n">
-        <v>0.9287355349196834</v>
+        <v>0.9435610710894989</v>
       </c>
       <c r="H10" t="n">
-        <v>1.0177066446734158</v>
+        <v>1.0360147936549124</v>
       </c>
       <c r="I10" t="n">
-        <v>1.1095734901044734</v>
+        <v>1.1308013356575952</v>
       </c>
       <c r="J10" t="n">
-        <v>1.2002074504988725</v>
-      </c>
-      <c r="K10" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="L10" t="e">
-        <v>#NUM!</v>
+        <v>1.2282618001805785</v>
+      </c>
+      <c r="K10" t="n">
+        <v>1.3285379784934344</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1.4313638577160734</v>
       </c>
     </row>
     <row r="11">
@@ -3491,34 +3551,34 @@
         <v>0.5</v>
       </c>
       <c r="C11" t="n">
-        <v>0.49595820946638686</v>
+        <v>0.5004777314014607</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4967414819875809</v>
+        <v>0.5069132785551892</v>
       </c>
       <c r="E11" t="n">
-        <v>0.503710830465092</v>
+        <v>0.519317406125767</v>
       </c>
       <c r="F11" t="n">
-        <v>0.5178455560495622</v>
+        <v>0.5376301729805513</v>
       </c>
       <c r="G11" t="n">
-        <v>0.5396245194667215</v>
+        <v>0.5616569204523728</v>
       </c>
       <c r="H11" t="n">
-        <v>0.5688239232760537</v>
+        <v>0.5909523851306558</v>
       </c>
       <c r="I11" t="n">
-        <v>0.6041300036879443</v>
+        <v>0.6247238645063495</v>
       </c>
       <c r="J11" t="n">
-        <v>0.639659025138353</v>
-      </c>
-      <c r="K11" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="L11" t="e">
-        <v>#NUM!</v>
+        <v>0.6620723359362585</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.7036605676547337</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.7579368499408234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Polynomials are approximated using polynomial regression
</commit_message>
<xml_diff>
--- a/resultBook.xlsx
+++ b/resultBook.xlsx
@@ -246,34 +246,28 @@
                   <c:v>0.7936507936507936</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7985175398975912</c:v>
+                  <c:v>0.7964671443145639</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.7999470240275934</c:v>
+                  <c:v>0.7906774682135947</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.7968687010880957</c:v>
+                  <c:v>0.7814381039512749</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.7880999397162711</c:v>
+                  <c:v>0.777841828637237</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.7723411720772755</c:v>
+                  <c:v>0.7922867964911615</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.7481814851195527</c:v>
+                  <c:v>0.8402330979296048</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.7141198053212</c:v>
+                  <c:v>0.94799791016554</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.6686209550437986</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.6102593894050423</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.5379563171798417</c:v>
+                  <c:v>1.3008905245729487</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -513,34 +507,28 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5004777314014607</c:v>
+                  <c:v>0.49595820946638425</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5069132785551892</c:v>
+                  <c:v>0.49674148198757523</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.519317406125767</c:v>
+                  <c:v>0.5037108304650835</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5376301729805513</c:v>
+                  <c:v>0.5178455560495503</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5616569204523728</c:v>
+                  <c:v>0.539624519466707</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5909523851306558</c:v>
+                  <c:v>0.5688239232760365</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.6247238645063495</c:v>
+                  <c:v>0.6041300036879272</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.6620723359362585</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.7036605676547337</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.7579368499408234</c:v>
+                  <c:v>0.6396590251383449</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -780,34 +768,28 @@
                   <c:v>0.6627906976744186</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6625592712483745</c:v>
+                  <c:v>0.6628295253534962</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6577605454001819</c:v>
+                  <c:v>0.663006218440504</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6478621622318</c:v>
+                  <c:v>0.6630935352519158</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.6323665658068801</c:v>
+                  <c:v>0.6639640597683897</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.610897288747511</c:v>
+                  <c:v>0.6679471918592815</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5833421956229687</c:v>
+                  <c:v>0.679575151038384</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5500761126945722</c:v>
+                  <c:v>0.7058480046218621</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.512299989687191</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.4725673618374788</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.4356465931125301</c:v>
+                  <c:v>0.7097351459341179</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1047,34 +1029,28 @@
                   <c:v>0.5581395348837209</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5193952492514508</c:v>
+                  <c:v>0.5099930956620913</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.47807060976512555</c:v>
+                  <c:v>0.45711599013229465</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.43276393224764764</c:v>
+                  <c:v>0.40607704333716504</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.38179996237145425</c:v>
+                  <c:v>0.36470317651973394</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.32320010514409264</c:v>
+                  <c:v>0.3406899078713379</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.25467405943894467</c:v>
+                  <c:v>0.3404923255650547</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.17366269217231584</c:v>
+                  <c:v>0.3716256617972899</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.07755608595454938</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-0.03546866382286415</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-0.16370879988422202</c:v>
+                  <c:v>0.49627489864770086</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1314,34 +1290,28 @@
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.30142108200324147</c:v>
+                  <c:v>0.3020070628335136</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.3527639360354631</c:v>
+                  <c:v>0.3542523085794068</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.40412602621681165</c:v>
+                  <c:v>0.4075166639982665</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.4556039878270791</c:v>
+                  <c:v>0.4615750624469502</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5071112501299861</c:v>
+                  <c:v>0.515170925893117</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5580512162527507</c:v>
+                  <c:v>0.5643871840916832</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.6067936876235762</c:v>
+                  <c:v>0.5984377770153521</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.6499005734600232</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.6810684722887468</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.6898376981702953</c:v>
+                  <c:v>0.6588468883788751</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1581,34 +1551,28 @@
                   <c:v>0.851063829787234</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8392756871350325</c:v>
+                  <c:v>0.8392883244104475</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8298855210392078</c:v>
+                  <c:v>0.8280065221462679</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.8233155257857421</c:v>
+                  <c:v>0.8170804974956407</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.8201712361188181</c:v>
+                  <c:v>0.8065108131163876</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.8213324531964666</c:v>
+                  <c:v>0.797218211420159</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.8280820115578699</c:v>
+                  <c:v>0.7914882516171455</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.842282767630592</c:v>
+                  <c:v>0.7926615351408527</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.866601550374608</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.9047093696348399</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.9610773304917004</c:v>
+                  <c:v>0.8105991436635933</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1848,34 +1812,28 @@
                   <c:v>0.8333333333333334</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.829903494774499</c:v>
+                  <c:v>0.8264785300783722</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8315816087477425</c:v>
+                  <c:v>0.8245404310007802</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.8397982646064193</c:v>
+                  <c:v>0.8283598582102396</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.8559663835764175</c:v>
+                  <c:v>0.8386558104572086</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.8815150662730444</c:v>
+                  <c:v>0.8561624135773356</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.9179192194199888</c:v>
+                  <c:v>0.8817507540953591</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.9667009099755334</c:v>
+                  <c:v>0.9162287135217525</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0293618520063987</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.107200167791253</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.2010108667157728</c:v>
+                  <c:v>0.9589327580386309</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2115,34 +2073,28 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.09999558493425532</c:v>
+                  <c:v>-0.09997666402937262</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.19990121713088746</c:v>
+                  <c:v>-0.1999575110026547</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.29968577862942636</c:v>
+                  <c:v>-0.2999219231562071</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.39934315648513025</c:v>
+                  <c:v>-0.3998419320349996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.4988979508479157</c:v>
+                  <c:v>-0.49969315389369456</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.598384589357363</c:v>
+                  <c:v>-0.5994563648821072</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.697794786347635</c:v>
+                  <c:v>-0.6990186661349361</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.7969972153746345</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-0.8956217756965511</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-0.9928278992206233</c:v>
+                  <c:v>-0.7977693459062928</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2382,34 +2334,28 @@
                   <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7804842244320525</c:v>
+                  <c:v>0.7840219905118377</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8619827917663819</c:v>
+                  <c:v>0.8656586752333428</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.9453887806576081</c:v>
+                  <c:v>0.942982931196805</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.031760661783467</c:v>
+                  <c:v>1.0141398597649185</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1224237026840023</c:v>
+                  <c:v>1.0778066029841034</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2190347556417933</c:v>
+                  <c:v>1.132994859131851</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3234177912581395</c:v>
+                  <c:v>1.18808449546574</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.4366816849518937</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.5567425212427146</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.6744069080591903</c:v>
+                  <c:v>1.3635740929948894</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2649,34 +2595,28 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5877714784914168</c:v>
+                  <c:v>0.5855114907477059</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6755758722216769</c:v>
+                  <c:v>0.6707727835243569</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.7638295634098229</c:v>
+                  <c:v>0.7560569160663637</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.852995107631085</c:v>
+                  <c:v>0.8418217979794852</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.9435610710894989</c:v>
+                  <c:v>0.9287355349196833</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0360147936549124</c:v>
+                  <c:v>1.017706644673415</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.1308013356575952</c:v>
+                  <c:v>1.109573490104472</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.2282618001805785</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.3285379784934344</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.4313638577160734</c:v>
+                  <c:v>1.200207450498878</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3209,34 +3149,34 @@
         <v>0.7936507936507936</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7985175398975912</v>
+        <v>0.7964671443145639</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7999470240275934</v>
+        <v>0.7906774682135947</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7968687010880957</v>
+        <v>0.7814381039512749</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7880999397162711</v>
+        <v>0.777841828637237</v>
       </c>
       <c r="G2" t="n">
-        <v>0.7723411720772755</v>
+        <v>0.7922867964911615</v>
       </c>
       <c r="H2" t="n">
-        <v>0.7481814851195527</v>
+        <v>0.8402330979296048</v>
       </c>
       <c r="I2" t="n">
-        <v>0.7141198053212</v>
+        <v>0.94799791016554</v>
       </c>
       <c r="J2" t="n">
-        <v>0.6686209550437986</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.6102593894050423</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.5379563171798417</v>
+        <v>1.3008905245729487</v>
+      </c>
+      <c r="K2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="L2" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="3">
@@ -3247,34 +3187,34 @@
         <v>0.6627906976744186</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6625592712483745</v>
+        <v>0.6628295253534962</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6577605454001819</v>
+        <v>0.663006218440504</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6478621622318</v>
+        <v>0.6630935352519158</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6323665658068801</v>
+        <v>0.6639640597683897</v>
       </c>
       <c r="G3" t="n">
-        <v>0.610897288747511</v>
+        <v>0.6679471918592815</v>
       </c>
       <c r="H3" t="n">
-        <v>0.5833421956229687</v>
+        <v>0.679575151038384</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5500761126945722</v>
+        <v>0.7058480046218621</v>
       </c>
       <c r="J3" t="n">
-        <v>0.512299989687191</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.4725673618374788</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.4356465931125301</v>
+        <v>0.7097351459341179</v>
+      </c>
+      <c r="K3" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="L3" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="4">
@@ -3285,34 +3225,34 @@
         <v>0.5581395348837209</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5193952492514508</v>
+        <v>0.5099930956620913</v>
       </c>
       <c r="D4" t="n">
-        <v>0.47807060976512555</v>
+        <v>0.45711599013229465</v>
       </c>
       <c r="E4" t="n">
-        <v>0.43276393224764764</v>
+        <v>0.40607704333716504</v>
       </c>
       <c r="F4" t="n">
-        <v>0.38179996237145425</v>
+        <v>0.36470317651973394</v>
       </c>
       <c r="G4" t="n">
-        <v>0.32320010514409264</v>
+        <v>0.3406899078713379</v>
       </c>
       <c r="H4" t="n">
-        <v>0.25467405943894467</v>
+        <v>0.3404923255650547</v>
       </c>
       <c r="I4" t="n">
-        <v>0.17366269217231584</v>
+        <v>0.3716256617972899</v>
       </c>
       <c r="J4" t="n">
-        <v>0.07755608595454938</v>
-      </c>
-      <c r="K4" t="n">
-        <v>-0.03546866382286415</v>
-      </c>
-      <c r="L4" t="n">
-        <v>-0.16370879988422202</v>
+        <v>0.49627489864770086</v>
+      </c>
+      <c r="K4" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="L4" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="5">
@@ -3323,34 +3263,34 @@
         <v>0.25</v>
       </c>
       <c r="C5" t="n">
-        <v>0.30142108200324147</v>
+        <v>0.3020070628335136</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3527639360354631</v>
+        <v>0.3542523085794068</v>
       </c>
       <c r="E5" t="n">
-        <v>0.40412602621681165</v>
+        <v>0.4075166639982665</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4556039878270791</v>
+        <v>0.4615750624469502</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5071112501299861</v>
+        <v>0.515170925893117</v>
       </c>
       <c r="H5" t="n">
-        <v>0.5580512162527507</v>
+        <v>0.5643871840916832</v>
       </c>
       <c r="I5" t="n">
-        <v>0.6067936876235762</v>
+        <v>0.5984377770153521</v>
       </c>
       <c r="J5" t="n">
-        <v>0.6499005734600232</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.6810684722887468</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.6898376981702953</v>
+        <v>0.6588468883788751</v>
+      </c>
+      <c r="K5" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="L5" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="6">
@@ -3361,34 +3301,34 @@
         <v>0.851063829787234</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8392756871350325</v>
+        <v>0.8392883244104475</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8298855210392078</v>
+        <v>0.8280065221462679</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8233155257857421</v>
+        <v>0.8170804974956407</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8201712361188181</v>
+        <v>0.8065108131163876</v>
       </c>
       <c r="G6" t="n">
-        <v>0.8213324531964666</v>
+        <v>0.797218211420159</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8280820115578699</v>
+        <v>0.7914882516171455</v>
       </c>
       <c r="I6" t="n">
-        <v>0.842282767630592</v>
+        <v>0.7926615351408527</v>
       </c>
       <c r="J6" t="n">
-        <v>0.866601550374608</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.9047093696348399</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.9610773304917004</v>
+        <v>0.8105991436635933</v>
+      </c>
+      <c r="K6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="L6" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="7">
@@ -3399,34 +3339,34 @@
         <v>0.8333333333333334</v>
       </c>
       <c r="C7" t="n">
-        <v>0.829903494774499</v>
+        <v>0.8264785300783722</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8315816087477425</v>
+        <v>0.8245404310007802</v>
       </c>
       <c r="E7" t="n">
-        <v>0.8397982646064193</v>
+        <v>0.8283598582102396</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8559663835764175</v>
+        <v>0.8386558104572086</v>
       </c>
       <c r="G7" t="n">
-        <v>0.8815150662730444</v>
+        <v>0.8561624135773356</v>
       </c>
       <c r="H7" t="n">
-        <v>0.9179192194199888</v>
+        <v>0.8817507540953591</v>
       </c>
       <c r="I7" t="n">
-        <v>0.9667009099755334</v>
+        <v>0.9162287135217525</v>
       </c>
       <c r="J7" t="n">
-        <v>1.0293618520063987</v>
-      </c>
-      <c r="K7" t="n">
-        <v>1.107200167791253</v>
-      </c>
-      <c r="L7" t="n">
-        <v>1.2010108667157728</v>
+        <v>0.9589327580386309</v>
+      </c>
+      <c r="K7" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="L7" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="8">
@@ -3437,34 +3377,34 @@
         <v>0.0</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.09999558493425532</v>
+        <v>-0.09997666402937262</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.19990121713088746</v>
+        <v>-0.1999575110026547</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.29968577862942636</v>
+        <v>-0.2999219231562071</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.39934315648513025</v>
+        <v>-0.3998419320349996</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.4988979508479157</v>
+        <v>-0.49969315389369456</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.598384589357363</v>
+        <v>-0.5994563648821072</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.697794786347635</v>
+        <v>-0.6990186661349361</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.7969972153746345</v>
-      </c>
-      <c r="K8" t="n">
-        <v>-0.8956217756965511</v>
-      </c>
-      <c r="L8" t="n">
-        <v>-0.9928278992206233</v>
+        <v>-0.7977693459062928</v>
+      </c>
+      <c r="K8" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="L8" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="9">
@@ -3475,34 +3415,34 @@
         <v>0.7</v>
       </c>
       <c r="C9" t="n">
-        <v>0.7804842244320525</v>
+        <v>0.7840219905118377</v>
       </c>
       <c r="D9" t="n">
-        <v>0.8619827917663819</v>
+        <v>0.8656586752333428</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9453887806576081</v>
+        <v>0.942982931196805</v>
       </c>
       <c r="F9" t="n">
-        <v>1.031760661783467</v>
+        <v>1.0141398597649185</v>
       </c>
       <c r="G9" t="n">
-        <v>1.1224237026840023</v>
+        <v>1.0778066029841034</v>
       </c>
       <c r="H9" t="n">
-        <v>1.2190347556417933</v>
+        <v>1.132994859131851</v>
       </c>
       <c r="I9" t="n">
-        <v>1.3234177912581395</v>
+        <v>1.18808449546574</v>
       </c>
       <c r="J9" t="n">
-        <v>1.4366816849518937</v>
-      </c>
-      <c r="K9" t="n">
-        <v>1.5567425212427146</v>
-      </c>
-      <c r="L9" t="n">
-        <v>1.6744069080591903</v>
+        <v>1.3635740929948894</v>
+      </c>
+      <c r="K9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="L9" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="10">
@@ -3513,34 +3453,34 @@
         <v>0.5</v>
       </c>
       <c r="C10" t="n">
-        <v>0.5877714784914168</v>
+        <v>0.5855114907477059</v>
       </c>
       <c r="D10" t="n">
-        <v>0.6755758722216769</v>
+        <v>0.6707727835243569</v>
       </c>
       <c r="E10" t="n">
-        <v>0.7638295634098229</v>
+        <v>0.7560569160663637</v>
       </c>
       <c r="F10" t="n">
-        <v>0.852995107631085</v>
+        <v>0.8418217979794852</v>
       </c>
       <c r="G10" t="n">
-        <v>0.9435610710894989</v>
+        <v>0.9287355349196833</v>
       </c>
       <c r="H10" t="n">
-        <v>1.0360147936549124</v>
+        <v>1.017706644673415</v>
       </c>
       <c r="I10" t="n">
-        <v>1.1308013356575952</v>
+        <v>1.109573490104472</v>
       </c>
       <c r="J10" t="n">
-        <v>1.2282618001805785</v>
-      </c>
-      <c r="K10" t="n">
-        <v>1.3285379784934344</v>
-      </c>
-      <c r="L10" t="n">
-        <v>1.4313638577160734</v>
+        <v>1.200207450498878</v>
+      </c>
+      <c r="K10" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="L10" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="11">
@@ -3551,34 +3491,34 @@
         <v>0.5</v>
       </c>
       <c r="C11" t="n">
-        <v>0.5004777314014607</v>
+        <v>0.49595820946638425</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5069132785551892</v>
+        <v>0.49674148198757523</v>
       </c>
       <c r="E11" t="n">
-        <v>0.519317406125767</v>
+        <v>0.5037108304650835</v>
       </c>
       <c r="F11" t="n">
-        <v>0.5376301729805513</v>
+        <v>0.5178455560495503</v>
       </c>
       <c r="G11" t="n">
-        <v>0.5616569204523728</v>
+        <v>0.539624519466707</v>
       </c>
       <c r="H11" t="n">
-        <v>0.5909523851306558</v>
+        <v>0.5688239232760365</v>
       </c>
       <c r="I11" t="n">
-        <v>0.6247238645063495</v>
+        <v>0.6041300036879272</v>
       </c>
       <c r="J11" t="n">
-        <v>0.6620723359362585</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0.7036605676547337</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0.7579368499408234</v>
+        <v>0.6396590251383449</v>
+      </c>
+      <c r="K11" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="L11" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some fixes for polynomial graphs
</commit_message>
<xml_diff>
--- a/resultBook.xlsx
+++ b/resultBook.xlsx
@@ -243,31 +243,31 @@
               <c:numCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.7936507936507936</c:v>
+                  <c:v>0.79</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7964671443145639</c:v>
+                  <c:v>0.7927836733069249</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.7906774682135947</c:v>
+                  <c:v>0.7869679203049471</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.7814381039512749</c:v>
+                  <c:v>0.777566187693712</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.777841828637237</c:v>
+                  <c:v>0.7736010745377082</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.7922867964911615</c:v>
+                  <c:v>0.7877679964003368</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.8402330979296048</c:v>
+                  <c:v>0.8368359125416572</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.94799791016554</c:v>
+                  <c:v>0.9499076749715731</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.3008905245729487</c:v>
+                  <c:v>1.3220088902680642</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -322,37 +322,37 @@
             <c:numLit>
               <c:ptCount val="11"/>
               <c:pt idx="0">
-                <c:v>0.7936507936507936</c:v>
+                <c:v>0.79</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>0.8095238095238095</c:v>
+                <c:v>0.81</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v>0.7301587301587301</c:v>
+                <c:v>0.73</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>0.746031746031746</c:v>
+                <c:v>0.75</c:v>
               </c:pt>
               <c:pt idx="4">
-                <c:v>0.8888888888888888</c:v>
+                <c:v>0.89</c:v>
               </c:pt>
               <c:pt idx="5">
                 <c:v>1.0</c:v>
               </c:pt>
               <c:pt idx="6">
-                <c:v>0.9206349206349206</c:v>
+                <c:v>0.92</c:v>
               </c:pt>
               <c:pt idx="7">
-                <c:v>0.9206349206349206</c:v>
+                <c:v>0.92</c:v>
               </c:pt>
               <c:pt idx="8">
-                <c:v>0.6507936507936508</c:v>
+                <c:v>0.65</c:v>
               </c:pt>
               <c:pt idx="9">
-                <c:v>0.7301587301587301</c:v>
+                <c:v>0.73</c:v>
               </c:pt>
               <c:pt idx="10">
-                <c:v>0.6190476190476191</c:v>
+                <c:v>0.62</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -507,28 +507,28 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.49595820946638425</c:v>
+                  <c:v>0.49612936322064227</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.49674148198757523</c:v>
+                  <c:v>0.49718515861620133</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5037108304650835</c:v>
+                  <c:v>0.5044352572242127</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5178455560495503</c:v>
+                  <c:v>0.5187461216717743</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.539624519466707</c:v>
+                  <c:v>0.5404424171251302</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5688239232760365</c:v>
+                  <c:v>0.569096987841909</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.6041300036879272</c:v>
+                  <c:v>0.6031928359778226</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.6396590251383449</c:v>
+                  <c:v>0.6367821389606265</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -765,31 +765,31 @@
               <c:numCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.6627906976744186</c:v>
+                  <c:v>0.66</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6628295253534962</c:v>
+                  <c:v>0.6596627345479693</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.663006218440504</c:v>
+                  <c:v>0.6597152283616166</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6630935352519158</c:v>
+                  <c:v>0.6599389551748343</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.6639640597683897</c:v>
+                  <c:v>0.6612460807579718</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.6679471918592815</c:v>
+                  <c:v>0.666046176042886</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.679575151038384</c:v>
+                  <c:v>0.6790937645891284</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.7058480046218621</c:v>
+                  <c:v>0.7079686445631489</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.7097351459341179</c:v>
+                  <c:v>0.7077055050662013</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -844,37 +844,37 @@
             <c:numLit>
               <c:ptCount val="11"/>
               <c:pt idx="0">
-                <c:v>0.6627906976744186</c:v>
+                <c:v>0.66</c:v>
               </c:pt>
               <c:pt idx="1">
                 <c:v>1.0</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v>0.7093023255813954</c:v>
+                <c:v>0.71</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>0.6976744186046512</c:v>
+                <c:v>0.7</c:v>
               </c:pt>
               <c:pt idx="4">
-                <c:v>0.9651162790697675</c:v>
+                <c:v>0.97</c:v>
               </c:pt>
               <c:pt idx="5">
-                <c:v>0.9302325581395349</c:v>
+                <c:v>0.93</c:v>
               </c:pt>
               <c:pt idx="6">
-                <c:v>0.9186046511627907</c:v>
+                <c:v>0.92</c:v>
               </c:pt>
               <c:pt idx="7">
-                <c:v>0.872093023255814</c:v>
+                <c:v>0.87</c:v>
               </c:pt>
               <c:pt idx="8">
-                <c:v>0.8255813953488372</c:v>
+                <c:v>0.83</c:v>
               </c:pt>
               <c:pt idx="9">
-                <c:v>0.813953488372093</c:v>
+                <c:v>0.81</c:v>
               </c:pt>
               <c:pt idx="10">
-                <c:v>0.813953488372093</c:v>
+                <c:v>0.81</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -1026,31 +1026,31 @@
               <c:numCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.5581395348837209</c:v>
+                  <c:v>0.56</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5099930956620913</c:v>
+                  <c:v>0.5118235756350319</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.45711599013229465</c:v>
+                  <c:v>0.45897696742120603</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.40607704333716504</c:v>
+                  <c:v>0.40811455375741984</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.36470317651973394</c:v>
+                  <c:v>0.3672106025433004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.3406899078713379</c:v>
+                  <c:v>0.3442367203741828</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.3404923255650547</c:v>
+                  <c:v>0.34614214790232334</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.3716256617972899</c:v>
+                  <c:v>0.3811997187327615</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.49627489864770086</c:v>
+                  <c:v>0.5172095189474274</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1105,37 +1105,37 @@
             <c:numLit>
               <c:ptCount val="11"/>
               <c:pt idx="0">
-                <c:v>0.5581395348837209</c:v>
+                <c:v>0.56</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>0.4418604651162791</c:v>
+                <c:v>0.44</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v>0.7674418604651163</c:v>
+                <c:v>0.77</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>0.5813953488372093</c:v>
+                <c:v>0.58</c:v>
               </c:pt>
               <c:pt idx="4">
-                <c:v>0.7906976744186046</c:v>
+                <c:v>0.79</c:v>
               </c:pt>
               <c:pt idx="5">
                 <c:v>1.0</c:v>
               </c:pt>
               <c:pt idx="6">
-                <c:v>0.8372093023255814</c:v>
+                <c:v>0.84</c:v>
               </c:pt>
               <c:pt idx="7">
-                <c:v>0.8837209302325582</c:v>
+                <c:v>0.88</c:v>
               </c:pt>
               <c:pt idx="8">
-                <c:v>0.5581395348837209</c:v>
+                <c:v>0.56</c:v>
               </c:pt>
               <c:pt idx="9">
-                <c:v>0.6046511627906976</c:v>
+                <c:v>0.6</c:v>
               </c:pt>
               <c:pt idx="10">
-                <c:v>0.5348837209302325</c:v>
+                <c:v>0.53</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -1290,28 +1290,28 @@
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.3020070628335136</c:v>
+                  <c:v>0.3026074442282167</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.3542523085794068</c:v>
+                  <c:v>0.3554573209492788</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.4075166639982665</c:v>
+                  <c:v>0.4093385132079238</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.4615750624469502</c:v>
+                  <c:v>0.4640320726784879</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.515170925893117</c:v>
+                  <c:v>0.5183120798953448</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5643871840916832</c:v>
+                  <c:v>0.5681560973251315</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5984377770153521</c:v>
+                  <c:v>0.6018964566326891</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.6588468883788751</c:v>
+                  <c:v>0.6775896805156523</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1375,19 +1375,19 @@
                 <c:v>0.35</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>0.6333333333333333</c:v>
+                <c:v>0.63</c:v>
               </c:pt>
               <c:pt idx="4">
-                <c:v>0.6666666666666666</c:v>
+                <c:v>0.67</c:v>
               </c:pt>
               <c:pt idx="5">
-                <c:v>0.7166666666666667</c:v>
+                <c:v>0.72</c:v>
               </c:pt>
               <c:pt idx="6">
-                <c:v>0.8333333333333334</c:v>
+                <c:v>0.83</c:v>
               </c:pt>
               <c:pt idx="7">
-                <c:v>0.9166666666666666</c:v>
+                <c:v>0.92</c:v>
               </c:pt>
               <c:pt idx="8">
                 <c:v>1.0</c:v>
@@ -1396,7 +1396,7 @@
                 <c:v>0.5</c:v>
               </c:pt>
               <c:pt idx="10">
-                <c:v>0.5833333333333334</c:v>
+                <c:v>0.58</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -1548,31 +1548,31 @@
               <c:numCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.851063829787234</c:v>
+                  <c:v>0.85</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8392883244104475</c:v>
+                  <c:v>0.8383710470625834</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8280065221462679</c:v>
+                  <c:v>0.827297752693395</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.8170804974956407</c:v>
+                  <c:v>0.8166309001043963</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.8065108131163876</c:v>
+                  <c:v>0.8063638624129827</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.797218211420159</c:v>
+                  <c:v>0.79743252410751</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.7914882516171455</c:v>
+                  <c:v>0.7921780703616438</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.7926615351408527</c:v>
+                  <c:v>0.7939491930490639</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.8105991436635933</c:v>
+                  <c:v>0.8122667893384697</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1627,37 +1627,37 @@
             <c:numLit>
               <c:ptCount val="11"/>
               <c:pt idx="0">
-                <c:v>0.851063829787234</c:v>
+                <c:v>0.85</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>0.851063829787234</c:v>
+                <c:v>0.85</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v>0.8829787234042553</c:v>
+                <c:v>0.88</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>0.8723404255319149</c:v>
+                <c:v>0.87</c:v>
               </c:pt>
               <c:pt idx="4">
-                <c:v>0.7446808510638298</c:v>
+                <c:v>0.74</c:v>
               </c:pt>
               <c:pt idx="5">
                 <c:v>1.0</c:v>
               </c:pt>
               <c:pt idx="6">
-                <c:v>0.851063829787234</c:v>
+                <c:v>0.85</c:v>
               </c:pt>
               <c:pt idx="7">
-                <c:v>0.7978723404255319</c:v>
+                <c:v>0.8</c:v>
               </c:pt>
               <c:pt idx="8">
-                <c:v>0.8191489361702128</c:v>
+                <c:v>0.82</c:v>
               </c:pt>
               <c:pt idx="9">
-                <c:v>0.851063829787234</c:v>
+                <c:v>0.85</c:v>
               </c:pt>
               <c:pt idx="10">
-                <c:v>0.7978723404255319</c:v>
+                <c:v>0.8</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -1809,31 +1809,31 @@
               <c:numCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.8333333333333334</c:v>
+                  <c:v>0.83</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8264785300783722</c:v>
+                  <c:v>0.8233066803350126</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8245404310007802</c:v>
+                  <c:v>0.8213462394354488</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.8283598582102396</c:v>
+                  <c:v>0.8249527120306893</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.8386558104572086</c:v>
+                  <c:v>0.8348512955835583</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.8561624135773356</c:v>
+                  <c:v>0.8517910637584998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.8817507540953591</c:v>
+                  <c:v>0.8766442575196696</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.9162287135217525</c:v>
+                  <c:v>0.9101445112779003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.9589327580386309</c:v>
+                  <c:v>0.9514533344727778</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1888,37 +1888,37 @@
             <c:numLit>
               <c:ptCount val="11"/>
               <c:pt idx="0">
-                <c:v>0.8333333333333334</c:v>
+                <c:v>0.83</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>0.8333333333333334</c:v>
+                <c:v>0.83</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v>0.625</c:v>
+                <c:v>0.63</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>0.6666666666666666</c:v>
+                <c:v>0.67</c:v>
               </c:pt>
               <c:pt idx="4">
                 <c:v>1.0</c:v>
               </c:pt>
               <c:pt idx="5">
-                <c:v>0.625</c:v>
+                <c:v>0.63</c:v>
               </c:pt>
               <c:pt idx="6">
-                <c:v>0.4166666666666667</c:v>
+                <c:v>0.42</c:v>
               </c:pt>
               <c:pt idx="7">
-                <c:v>0.7916666666666666</c:v>
+                <c:v>0.79</c:v>
               </c:pt>
               <c:pt idx="8">
-                <c:v>0.875</c:v>
+                <c:v>0.88</c:v>
               </c:pt>
               <c:pt idx="9">
-                <c:v>0.6666666666666666</c:v>
+                <c:v>0.67</c:v>
               </c:pt>
               <c:pt idx="10">
-                <c:v>0.8333333333333334</c:v>
+                <c:v>0.83</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -2073,28 +2073,28 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.09997666402937262</c:v>
+                  <c:v>-0.09997574815657335</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.1999575110026547</c:v>
+                  <c:v>-0.1999548168340894</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.2999219231562071</c:v>
+                  <c:v>-0.29991529252772836</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.3998419320349996</c:v>
+                  <c:v>-0.3998284711768813</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.49969315389369456</c:v>
+                  <c:v>-0.4996739507859781</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.5994563648821072</c:v>
+                  <c:v>-0.5994495112785021</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.6990186661349361</c:v>
+                  <c:v>-0.6990854000724319</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.7977693459062928</c:v>
+                  <c:v>-0.7980558764895072</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2155,7 +2155,7 @@
                 <c:v>0.0</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v>0.375</c:v>
+                <c:v>0.38</c:v>
               </c:pt>
               <c:pt idx="3">
                 <c:v>0.55</c:v>
@@ -2164,7 +2164,7 @@
                 <c:v>0.2</c:v>
               </c:pt>
               <c:pt idx="5">
-                <c:v>0.775</c:v>
+                <c:v>0.78</c:v>
               </c:pt>
               <c:pt idx="6">
                 <c:v>1.0</c:v>
@@ -2176,7 +2176,7 @@
                 <c:v>0.0</c:v>
               </c:pt>
               <c:pt idx="9">
-                <c:v>0.125</c:v>
+                <c:v>0.13</c:v>
               </c:pt>
               <c:pt idx="10">
                 <c:v>0.35</c:v>
@@ -2334,28 +2334,28 @@
                   <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7840219905118377</c:v>
+                  <c:v>0.7842788816094669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8656586752333428</c:v>
+                  <c:v>0.8662199491765333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.942982931196805</c:v>
+                  <c:v>0.9439868096590878</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0141398597649185</c:v>
+                  <c:v>1.015852000267118</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0778066029841034</c:v>
+                  <c:v>1.0806871092775912</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.132994859131851</c:v>
+                  <c:v>1.1375700038665932</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.18808449546574</c:v>
+                  <c:v>1.1945300855488215</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.3635740929948894</c:v>
+                  <c:v>1.3779591773700006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2595,28 +2595,28 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5855114907477059</c:v>
+                  <c:v>0.5853177205033419</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6707727835243569</c:v>
+                  <c:v>0.6703989035094037</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.7560569160663637</c:v>
+                  <c:v>0.7555098102594294</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.8418217979794852</c:v>
+                  <c:v>0.8410936501480445</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.9287355349196833</c:v>
+                  <c:v>0.9277894807551238</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.017706644673415</c:v>
+                  <c:v>1.0164829522537466</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.109573490104472</c:v>
+                  <c:v>1.1080348001448395</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.200207450498878</c:v>
+                  <c:v>1.1970337221557672</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3146,31 +3146,31 @@
         <v>11</v>
       </c>
       <c r="B2" t="n">
-        <v>0.7936507936507936</v>
+        <v>0.79</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7964671443145639</v>
+        <v>0.7927836733069249</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7906774682135947</v>
+        <v>0.7869679203049471</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7814381039512749</v>
+        <v>0.777566187693712</v>
       </c>
       <c r="F2" t="n">
-        <v>0.777841828637237</v>
+        <v>0.7736010745377082</v>
       </c>
       <c r="G2" t="n">
-        <v>0.7922867964911615</v>
+        <v>0.7877679964003368</v>
       </c>
       <c r="H2" t="n">
-        <v>0.8402330979296048</v>
+        <v>0.8368359125416572</v>
       </c>
       <c r="I2" t="n">
-        <v>0.94799791016554</v>
+        <v>0.9499076749715731</v>
       </c>
       <c r="J2" t="n">
-        <v>1.3008905245729487</v>
+        <v>1.3220088902680642</v>
       </c>
       <c r="K2" t="e">
         <v>#NUM!</v>
@@ -3184,31 +3184,31 @@
         <v>12</v>
       </c>
       <c r="B3" t="n">
-        <v>0.6627906976744186</v>
+        <v>0.66</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6628295253534962</v>
+        <v>0.6596627345479693</v>
       </c>
       <c r="D3" t="n">
-        <v>0.663006218440504</v>
+        <v>0.6597152283616166</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6630935352519158</v>
+        <v>0.6599389551748343</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6639640597683897</v>
+        <v>0.6612460807579718</v>
       </c>
       <c r="G3" t="n">
-        <v>0.6679471918592815</v>
+        <v>0.666046176042886</v>
       </c>
       <c r="H3" t="n">
-        <v>0.679575151038384</v>
+        <v>0.6790937645891284</v>
       </c>
       <c r="I3" t="n">
-        <v>0.7058480046218621</v>
+        <v>0.7079686445631489</v>
       </c>
       <c r="J3" t="n">
-        <v>0.7097351459341179</v>
+        <v>0.7077055050662013</v>
       </c>
       <c r="K3" t="e">
         <v>#NUM!</v>
@@ -3222,31 +3222,31 @@
         <v>13</v>
       </c>
       <c r="B4" t="n">
-        <v>0.5581395348837209</v>
+        <v>0.56</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5099930956620913</v>
+        <v>0.5118235756350319</v>
       </c>
       <c r="D4" t="n">
-        <v>0.45711599013229465</v>
+        <v>0.45897696742120603</v>
       </c>
       <c r="E4" t="n">
-        <v>0.40607704333716504</v>
+        <v>0.40811455375741984</v>
       </c>
       <c r="F4" t="n">
-        <v>0.36470317651973394</v>
+        <v>0.3672106025433004</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3406899078713379</v>
+        <v>0.3442367203741828</v>
       </c>
       <c r="H4" t="n">
-        <v>0.3404923255650547</v>
+        <v>0.34614214790232334</v>
       </c>
       <c r="I4" t="n">
-        <v>0.3716256617972899</v>
+        <v>0.3811997187327615</v>
       </c>
       <c r="J4" t="n">
-        <v>0.49627489864770086</v>
+        <v>0.5172095189474274</v>
       </c>
       <c r="K4" t="e">
         <v>#NUM!</v>
@@ -3263,28 +3263,28 @@
         <v>0.25</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3020070628335136</v>
+        <v>0.3026074442282167</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3542523085794068</v>
+        <v>0.3554573209492788</v>
       </c>
       <c r="E5" t="n">
-        <v>0.4075166639982665</v>
+        <v>0.4093385132079238</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4615750624469502</v>
+        <v>0.4640320726784879</v>
       </c>
       <c r="G5" t="n">
-        <v>0.515170925893117</v>
+        <v>0.5183120798953448</v>
       </c>
       <c r="H5" t="n">
-        <v>0.5643871840916832</v>
+        <v>0.5681560973251315</v>
       </c>
       <c r="I5" t="n">
-        <v>0.5984377770153521</v>
+        <v>0.6018964566326891</v>
       </c>
       <c r="J5" t="n">
-        <v>0.6588468883788751</v>
+        <v>0.6775896805156523</v>
       </c>
       <c r="K5" t="e">
         <v>#NUM!</v>
@@ -3298,31 +3298,31 @@
         <v>15</v>
       </c>
       <c r="B6" t="n">
-        <v>0.851063829787234</v>
+        <v>0.85</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8392883244104475</v>
+        <v>0.8383710470625834</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8280065221462679</v>
+        <v>0.827297752693395</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8170804974956407</v>
+        <v>0.8166309001043963</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8065108131163876</v>
+        <v>0.8063638624129827</v>
       </c>
       <c r="G6" t="n">
-        <v>0.797218211420159</v>
+        <v>0.79743252410751</v>
       </c>
       <c r="H6" t="n">
-        <v>0.7914882516171455</v>
+        <v>0.7921780703616438</v>
       </c>
       <c r="I6" t="n">
-        <v>0.7926615351408527</v>
+        <v>0.7939491930490639</v>
       </c>
       <c r="J6" t="n">
-        <v>0.8105991436635933</v>
+        <v>0.8122667893384697</v>
       </c>
       <c r="K6" t="e">
         <v>#NUM!</v>
@@ -3336,31 +3336,31 @@
         <v>16</v>
       </c>
       <c r="B7" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.83</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8264785300783722</v>
+        <v>0.8233066803350126</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8245404310007802</v>
+        <v>0.8213462394354488</v>
       </c>
       <c r="E7" t="n">
-        <v>0.8283598582102396</v>
+        <v>0.8249527120306893</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8386558104572086</v>
+        <v>0.8348512955835583</v>
       </c>
       <c r="G7" t="n">
-        <v>0.8561624135773356</v>
+        <v>0.8517910637584998</v>
       </c>
       <c r="H7" t="n">
-        <v>0.8817507540953591</v>
+        <v>0.8766442575196696</v>
       </c>
       <c r="I7" t="n">
-        <v>0.9162287135217525</v>
+        <v>0.9101445112779003</v>
       </c>
       <c r="J7" t="n">
-        <v>0.9589327580386309</v>
+        <v>0.9514533344727778</v>
       </c>
       <c r="K7" t="e">
         <v>#NUM!</v>
@@ -3377,28 +3377,28 @@
         <v>0.0</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.09997666402937262</v>
+        <v>-0.09997574815657335</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.1999575110026547</v>
+        <v>-0.1999548168340894</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.2999219231562071</v>
+        <v>-0.29991529252772836</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.3998419320349996</v>
+        <v>-0.3998284711768813</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.49969315389369456</v>
+        <v>-0.4996739507859781</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.5994563648821072</v>
+        <v>-0.5994495112785021</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.6990186661349361</v>
+        <v>-0.6990854000724319</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.7977693459062928</v>
+        <v>-0.7980558764895072</v>
       </c>
       <c r="K8" t="e">
         <v>#NUM!</v>
@@ -3415,28 +3415,28 @@
         <v>0.7</v>
       </c>
       <c r="C9" t="n">
-        <v>0.7840219905118377</v>
+        <v>0.7842788816094669</v>
       </c>
       <c r="D9" t="n">
-        <v>0.8656586752333428</v>
+        <v>0.8662199491765333</v>
       </c>
       <c r="E9" t="n">
-        <v>0.942982931196805</v>
+        <v>0.9439868096590878</v>
       </c>
       <c r="F9" t="n">
-        <v>1.0141398597649185</v>
+        <v>1.015852000267118</v>
       </c>
       <c r="G9" t="n">
-        <v>1.0778066029841034</v>
+        <v>1.0806871092775912</v>
       </c>
       <c r="H9" t="n">
-        <v>1.132994859131851</v>
+        <v>1.1375700038665932</v>
       </c>
       <c r="I9" t="n">
-        <v>1.18808449546574</v>
+        <v>1.1945300855488215</v>
       </c>
       <c r="J9" t="n">
-        <v>1.3635740929948894</v>
+        <v>1.3779591773700006</v>
       </c>
       <c r="K9" t="e">
         <v>#NUM!</v>
@@ -3453,28 +3453,28 @@
         <v>0.5</v>
       </c>
       <c r="C10" t="n">
-        <v>0.5855114907477059</v>
+        <v>0.5853177205033419</v>
       </c>
       <c r="D10" t="n">
-        <v>0.6707727835243569</v>
+        <v>0.6703989035094037</v>
       </c>
       <c r="E10" t="n">
-        <v>0.7560569160663637</v>
+        <v>0.7555098102594294</v>
       </c>
       <c r="F10" t="n">
-        <v>0.8418217979794852</v>
+        <v>0.8410936501480445</v>
       </c>
       <c r="G10" t="n">
-        <v>0.9287355349196833</v>
+        <v>0.9277894807551238</v>
       </c>
       <c r="H10" t="n">
-        <v>1.017706644673415</v>
+        <v>1.0164829522537466</v>
       </c>
       <c r="I10" t="n">
-        <v>1.109573490104472</v>
+        <v>1.1080348001448395</v>
       </c>
       <c r="J10" t="n">
-        <v>1.200207450498878</v>
+        <v>1.1970337221557672</v>
       </c>
       <c r="K10" t="e">
         <v>#NUM!</v>
@@ -3491,28 +3491,28 @@
         <v>0.5</v>
       </c>
       <c r="C11" t="n">
-        <v>0.49595820946638425</v>
+        <v>0.49612936322064227</v>
       </c>
       <c r="D11" t="n">
-        <v>0.49674148198757523</v>
+        <v>0.49718515861620133</v>
       </c>
       <c r="E11" t="n">
-        <v>0.5037108304650835</v>
+        <v>0.5044352572242127</v>
       </c>
       <c r="F11" t="n">
-        <v>0.5178455560495503</v>
+        <v>0.5187461216717743</v>
       </c>
       <c r="G11" t="n">
-        <v>0.539624519466707</v>
+        <v>0.5404424171251302</v>
       </c>
       <c r="H11" t="n">
-        <v>0.5688239232760365</v>
+        <v>0.569096987841909</v>
       </c>
       <c r="I11" t="n">
-        <v>0.6041300036879272</v>
+        <v>0.6031928359778226</v>
       </c>
       <c r="J11" t="n">
-        <v>0.6396590251383449</v>
+        <v>0.6367821389606265</v>
       </c>
       <c r="K11" t="e">
         <v>#NUM!</v>

</xml_diff>